<commit_message>
added county data and highlighted items that may need more work to merge
</commit_message>
<xml_diff>
--- a/US-data-only-green-area-per_capita-square-meters-per-capita.xlsx
+++ b/US-data-only-green-area-per_capita-square-meters-per-capita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody\Documents\Data Bootcamp\WUSTL-Bootcamp\project 3\Project3-Greenspace-Health\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29C1F228-5143-4BDD-B9D2-DDC261263E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13525B6A-7D61-4DEF-B246-8F470E5BCE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,49 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="126">
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Data  Source</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: OECD.Stat</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>Note:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Green area per capita is calculated from Green area per million people and city population data source from OECD.</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="124">
   <si>
     <t>percent change</t>
   </si>
@@ -454,7 +412,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,14 +432,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -605,42 +555,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -952,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,10 +915,10 @@
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="6">
         <v>2000</v>
@@ -1016,15 +966,15 @@
         <v>2014</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="8">
         <v>1516.5716376399998</v>
@@ -1078,9 +1028,9 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="13"/>
+        <v>4</v>
+      </c>
+      <c r="B3" s="12"/>
       <c r="C3" s="7">
         <v>3186.4004016999997</v>
       </c>
@@ -1133,10 +1083,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="8">
         <v>12.661971209999999</v>
@@ -1190,10 +1140,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" s="7">
         <v>964.24896096000009</v>
@@ -1247,10 +1197,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="C6" s="8">
         <v>1939.65870238</v>
@@ -1304,10 +1254,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>76</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="C7" s="7">
         <v>6291.6493528400006</v>
@@ -1361,9 +1311,9 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="13"/>
+        <v>9</v>
+      </c>
+      <c r="B8" s="12"/>
       <c r="C8" s="8">
         <v>5865.7684442399996</v>
       </c>
@@ -1416,10 +1366,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>77</v>
+        <v>10</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="C9" s="7">
         <v>8672.4290523199998</v>
@@ -1473,10 +1423,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>123</v>
+        <v>71</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>121</v>
       </c>
       <c r="C10" s="8">
         <v>4764.1408880700001</v>
@@ -1530,10 +1480,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11" s="7">
         <v>126.21123567999999</v>
@@ -1587,10 +1537,10 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C12" s="8">
         <v>9833.0861384199998</v>
@@ -1644,10 +1594,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" s="7">
         <v>162.28689578999999</v>
@@ -1701,10 +1651,10 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="8">
         <v>90.129984959999987</v>
@@ -1758,10 +1708,10 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>80</v>
+        <v>15</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="C15" s="7">
         <v>466.88327296000006</v>
@@ -1815,10 +1765,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C16" s="8">
         <v>38.432583990000005</v>
@@ -1872,10 +1822,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="C17" s="7">
         <v>895.32488619000003</v>
@@ -1929,10 +1879,10 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="8">
         <v>33.25950606</v>
@@ -1986,10 +1936,10 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>82</v>
+        <v>19</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="C19" s="7">
         <v>3856.7927781900003</v>
@@ -2043,10 +1993,10 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C20" s="8">
         <v>294.72102254000004</v>
@@ -2100,10 +2050,10 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>84</v>
+        <v>21</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="C21" s="7">
         <v>989.79548346000001</v>
@@ -2157,10 +2107,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22" s="8">
         <v>818.0857306800001</v>
@@ -2214,10 +2164,10 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>86</v>
+        <v>23</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="C23" s="7">
         <v>275.19216210000002</v>
@@ -2271,10 +2221,10 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C24" s="8">
         <v>2475.8774795700001</v>
@@ -2328,10 +2278,10 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>87</v>
+        <v>25</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="C25" s="7">
         <v>2096.9824208700002</v>
@@ -2385,10 +2335,10 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>88</v>
+        <v>26</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="C26" s="8">
         <v>317.03907119999997</v>
@@ -2442,10 +2392,10 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>89</v>
+        <v>27</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="C27" s="7">
         <v>3970.9600181999999</v>
@@ -2499,10 +2449,10 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C28" s="8">
         <v>767.40209902999993</v>
@@ -2556,10 +2506,10 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C29" s="7">
         <v>658.36417210000002</v>
@@ -2613,10 +2563,10 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C30" s="8">
         <v>2185.0087031500002</v>
@@ -2670,10 +2620,10 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>92</v>
+        <v>31</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>90</v>
       </c>
       <c r="C31" s="7">
         <v>1712.11265293</v>
@@ -2727,10 +2677,10 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>93</v>
+        <v>32</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>91</v>
       </c>
       <c r="C32" s="8">
         <v>776.63186436000001</v>
@@ -2784,10 +2734,10 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>54</v>
+        <v>33</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C33" s="7">
         <v>10.30356828</v>
@@ -2841,10 +2791,10 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>94</v>
+        <v>34</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="C34" s="8">
         <v>5172.6287596500006</v>
@@ -2898,10 +2848,10 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>95</v>
+        <v>35</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="C35" s="7">
         <v>24.47098162</v>
@@ -2955,10 +2905,10 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C36" s="8">
         <v>107.32979520000001</v>
@@ -3012,9 +2962,9 @@
     </row>
     <row r="37" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="13"/>
+        <v>37</v>
+      </c>
+      <c r="B37" s="12"/>
       <c r="C37" s="7">
         <v>816.35101197999995</v>
       </c>
@@ -3067,10 +3017,10 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C38" s="8">
         <v>87.58366903999999</v>
@@ -3124,10 +3074,10 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>98</v>
+        <v>39</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="C39" s="7">
         <v>3.2248925000000002</v>
@@ -3181,10 +3131,10 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>99</v>
+        <v>40</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="C40" s="8">
         <v>5360.45563408</v>
@@ -3238,10 +3188,10 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C41" s="7">
         <v>2050.4191095300002</v>
@@ -3295,10 +3245,10 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C42" s="8">
         <v>1853.3654306199999</v>
@@ -3352,10 +3302,10 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C43" s="7">
         <v>164.6417763</v>
@@ -3409,10 +3359,10 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>102</v>
+        <v>44</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="C44" s="8">
         <v>1020.0617648199999</v>
@@ -3466,10 +3416,10 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C45" s="7">
         <v>60.750575740000002</v>
@@ -3523,10 +3473,10 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>104</v>
+        <v>46</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="C46" s="8">
         <v>4058.9822880000002</v>
@@ -3580,10 +3530,10 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>105</v>
+        <v>47</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="C47" s="7">
         <v>1884.4881833999998</v>
@@ -3637,9 +3587,9 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="13"/>
+        <v>48</v>
+      </c>
+      <c r="B48" s="12"/>
       <c r="C48" s="8">
         <v>137.59683858</v>
       </c>
@@ -3692,10 +3642,10 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>94</v>
+        <v>70</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="C49" s="7">
         <v>1088.10466204</v>
@@ -3749,10 +3699,10 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C50" s="8">
         <v>45.289410140000001</v>
@@ -3806,10 +3756,10 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C51" s="7">
         <v>302.88503510999993</v>
@@ -3863,10 +3813,10 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C52" s="8">
         <v>1.07155742</v>
@@ -3920,10 +3870,10 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C53" s="7">
         <v>3.0050504000000005</v>
@@ -3977,10 +3927,10 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C54" s="8">
         <v>542.65678322999997</v>
@@ -4034,10 +3984,10 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C55" s="7">
         <v>276.69752819999997</v>
@@ -4091,10 +4041,10 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>110</v>
+        <v>55</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C56" s="8">
         <v>217.45421999999999</v>
@@ -4148,10 +4098,10 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C57" s="7">
         <v>238.9178636</v>
@@ -4205,10 +4155,10 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C58" s="8">
         <v>384.67317613000006</v>
@@ -4262,10 +4212,10 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>112</v>
+        <v>58</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="C59" s="7">
         <v>567.77207476000001</v>
@@ -4319,10 +4269,10 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>113</v>
+        <v>59</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="C60" s="8">
         <v>108.40297668000001</v>
@@ -4376,10 +4326,10 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C61" s="7">
         <v>2698.2594209200001</v>
@@ -4433,10 +4383,10 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>115</v>
+        <v>61</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="C62" s="8">
         <v>2640.9405270000002</v>
@@ -4490,10 +4440,10 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>116</v>
+        <v>62</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="C63" s="7">
         <v>1688.7172005</v>
@@ -4547,10 +4497,10 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="C64" s="8">
         <v>1601.7845625</v>
@@ -4604,10 +4554,10 @@
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C65" s="7">
         <v>103.68367020000001</v>
@@ -4661,10 +4611,10 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>117</v>
+        <v>72</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="C66" s="8">
         <v>253.08283263999999</v>
@@ -4718,10 +4668,10 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>118</v>
+        <v>65</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="C67" s="7">
         <v>3023.4678466799996</v>
@@ -4775,10 +4725,10 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B68" s="12" t="s">
-        <v>119</v>
+        <v>66</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>117</v>
       </c>
       <c r="C68" s="8">
         <v>638.82242644000007</v>
@@ -4832,10 +4782,10 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69" s="12" t="s">
-        <v>120</v>
+        <v>67</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>118</v>
       </c>
       <c r="C69" s="7">
         <v>696.78372155000011</v>
@@ -4889,10 +4839,10 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C70" s="8">
         <v>630.23997652000003</v>
@@ -4946,10 +4896,10 @@
     </row>
     <row r="71" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C71" s="9">
         <v>754.31170764000001</v>
@@ -5002,9 +4952,6 @@
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>0</v>
-      </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -5022,22 +4969,20 @@
       <c r="Q72" s="1"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="11"/>
-      <c r="K74" s="11"/>
-      <c r="L74" s="11"/>
-      <c r="M74" s="11"/>
-      <c r="N74" s="11"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
+      <c r="M74" s="13"/>
+      <c r="N74" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
added average greenspace column to account for largely static data
</commit_message>
<xml_diff>
--- a/US-data-only-green-area-per_capita-square-meters-per-capita.xlsx
+++ b/US-data-only-green-area-per_capita-square-meters-per-capita.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody\Documents\Data Bootcamp\WUSTL-Bootcamp\project 3\Project3-Greenspace-Health\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CBA42F-7728-42B0-8665-077731844731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DC382E-648B-47C4-AE23-299986D842D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="5040" windowWidth="24060" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9585" yWindow="4800" windowWidth="26490" windowHeight="14565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Green area" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="157">
   <si>
     <t>county</t>
   </si>
@@ -499,6 +499,9 @@
   </si>
   <si>
     <t>UT</t>
+  </si>
+  <si>
+    <t>average_greenspace</t>
   </si>
 </sst>
 </file>
@@ -647,7 +650,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -679,6 +682,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -987,20 +991,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S70"/>
+  <dimension ref="A1:T70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A48" activeCellId="3" sqref="A8:XFD8 A3:XFD3 A37:XFD37 A48:XFD48"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="26.140625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>119</v>
       </c>
@@ -1058,8 +1063,11 @@
       <c r="S1" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1115,11 +1123,15 @@
         <v>1516.56055072</v>
       </c>
       <c r="S2" s="10">
-        <f t="shared" ref="S2:S18" si="0">(D2-R2)/D2</f>
-        <v>7.3105151940271317E-6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <f>(R2-D2)/D2</f>
+        <v>-7.3105151940271317E-6</v>
+      </c>
+      <c r="T2" s="13">
+        <f>AVERAGE(D2:R2)</f>
+        <v>1516.5645661173335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1175,11 +1187,15 @@
         <v>12.677987999999999</v>
       </c>
       <c r="S3" s="10">
-        <f t="shared" si="0"/>
-        <v>-1.2649523312255355E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" ref="S3:S66" si="0">(R3-D3)/D3</f>
+        <v>1.2649523312255355E-3</v>
+      </c>
+      <c r="T3" s="13">
+        <f t="shared" ref="T3:T66" si="1">AVERAGE(D3:R3)</f>
+        <v>12.66510854</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1236,10 +1252,14 @@
       </c>
       <c r="S4" s="10">
         <f t="shared" si="0"/>
-        <v>1.4054129741140164E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>-1.4054129741140164E-5</v>
+      </c>
+      <c r="T4" s="13">
+        <f t="shared" si="1"/>
+        <v>964.24774196733335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1296,10 +1316,14 @@
       </c>
       <c r="S5" s="10">
         <f t="shared" si="0"/>
-        <v>5.696043322654424E-6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>-5.696043322654424E-6</v>
+      </c>
+      <c r="T5" s="13">
+        <f t="shared" si="1"/>
+        <v>1939.6559161466669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1356,10 +1380,14 @@
       </c>
       <c r="S6" s="10">
         <f t="shared" si="0"/>
-        <v>1.3119548687691538E-6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>-1.3119548687691538E-6</v>
+      </c>
+      <c r="T6" s="13">
+        <f t="shared" si="1"/>
+        <v>6291.645367012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1416,10 +1444,14 @@
       </c>
       <c r="S7" s="10">
         <f t="shared" si="0"/>
-        <v>4.0422354320219692E-7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>-4.0422354320219692E-7</v>
+      </c>
+      <c r="T7" s="13">
+        <f t="shared" si="1"/>
+        <v>8672.4257482406665</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>65</v>
       </c>
@@ -1476,10 +1508,14 @@
       </c>
       <c r="S8" s="10">
         <f t="shared" si="0"/>
-        <v>2.9539281752459483E-6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+        <v>-2.9539281752459483E-6</v>
+      </c>
+      <c r="T8" s="13">
+        <f t="shared" si="1"/>
+        <v>4764.1349448786659</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1536,10 +1572,14 @@
       </c>
       <c r="S9" s="10">
         <f t="shared" si="0"/>
-        <v>-6.917704238437088E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>6.917704238437088E-5</v>
+      </c>
+      <c r="T9" s="13">
+        <f t="shared" si="1"/>
+        <v>126.216784264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1596,10 +1636,14 @@
       </c>
       <c r="S10" s="10">
         <f t="shared" si="0"/>
-        <v>-5.0354486175636275E-7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <v>5.0354486175636275E-7</v>
+      </c>
+      <c r="T10" s="13">
+        <f t="shared" si="1"/>
+        <v>9833.0881462999987</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1656,10 +1700,14 @@
       </c>
       <c r="S11" s="10">
         <f t="shared" si="0"/>
-        <v>-4.5680767777918204E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>4.5680767777918204E-5</v>
+      </c>
+      <c r="T11" s="13">
+        <f t="shared" si="1"/>
+        <v>162.28310052999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1716,10 +1764,14 @@
       </c>
       <c r="S12" s="10">
         <f t="shared" si="0"/>
-        <v>-6.5463519189756195E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>6.5463519189756195E-4</v>
+      </c>
+      <c r="T12" s="13">
+        <f t="shared" si="1"/>
+        <v>90.162653249999977</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1776,10 +1828,14 @@
       </c>
       <c r="S13" s="10">
         <f t="shared" si="0"/>
-        <v>2.580088150114906E-6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+        <v>-2.580088150114906E-6</v>
+      </c>
+      <c r="T13" s="13">
+        <f t="shared" si="1"/>
+        <v>466.87880266999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1836,10 +1892,14 @@
       </c>
       <c r="S14" s="10">
         <f t="shared" si="0"/>
-        <v>1.0373073018036272E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+        <v>-1.0373073018036272E-4</v>
+      </c>
+      <c r="T14" s="13">
+        <f t="shared" si="1"/>
+        <v>38.427154561333332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1896,10 +1956,14 @@
       </c>
       <c r="S15" s="10">
         <f t="shared" si="0"/>
-        <v>-2.494961364813236E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+        <v>2.494961364813236E-5</v>
+      </c>
+      <c r="T15" s="13">
+        <f t="shared" si="1"/>
+        <v>895.34107569599996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1956,10 +2020,14 @@
       </c>
       <c r="S16" s="10">
         <f t="shared" si="0"/>
-        <v>-6.7159415896624042E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+        <v>6.7159415896624042E-4</v>
+      </c>
+      <c r="T16" s="13">
+        <f t="shared" si="1"/>
+        <v>33.272976707333342</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -2016,10 +2084,14 @@
       </c>
       <c r="S17" s="10">
         <f t="shared" si="0"/>
-        <v>1.4983874769257437E-6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+        <v>-1.4983874769257437E-6</v>
+      </c>
+      <c r="T17" s="13">
+        <f t="shared" si="1"/>
+        <v>3856.773289863333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -2076,10 +2148,14 @@
       </c>
       <c r="S18" s="10">
         <f t="shared" si="0"/>
-        <v>1.1893756237171344E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+        <v>-1.1893756237171344E-5</v>
+      </c>
+      <c r="T18" s="13">
+        <f t="shared" si="1"/>
+        <v>294.72719920666663</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2135,11 +2211,15 @@
         <v>989.79730959999995</v>
       </c>
       <c r="S19" s="10">
-        <f t="shared" ref="S19:S67" si="1">(D19-R19)/D19</f>
-        <v>-1.8449669961627362E-6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.8449669961627362E-6</v>
+      </c>
+      <c r="T19" s="13">
+        <f t="shared" si="1"/>
+        <v>989.78993809266649</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -2195,11 +2275,15 @@
         <v>818.04891470000007</v>
       </c>
       <c r="S20" s="10">
-        <f t="shared" si="1"/>
-        <v>4.5002594006164528E-5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-4.5002594006164528E-5</v>
+      </c>
+      <c r="T20" s="13">
+        <f t="shared" si="1"/>
+        <v>818.06768844466671</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -2255,11 +2339,15 @@
         <v>275.19667646999994</v>
       </c>
       <c r="S21" s="10">
-        <f t="shared" si="1"/>
-        <v>-1.6404427965807907E-5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.6404427965807907E-5</v>
+      </c>
+      <c r="T21" s="13">
+        <f t="shared" si="1"/>
+        <v>275.19221146000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -2315,11 +2403,15 @@
         <v>2475.8699876000001</v>
       </c>
       <c r="S22" s="10">
-        <f t="shared" si="1"/>
-        <v>3.0259857613582702E-6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-3.0259857613582702E-6</v>
+      </c>
+      <c r="T22" s="13">
+        <f t="shared" si="1"/>
+        <v>2475.8735380140006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -2375,11 +2467,15 @@
         <v>2096.9864888699999</v>
       </c>
       <c r="S23" s="10">
-        <f t="shared" si="1"/>
-        <v>-1.9399304253804804E-6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.9399304253804804E-6</v>
+      </c>
+      <c r="T23" s="13">
+        <f t="shared" si="1"/>
+        <v>2096.9975485813334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -2435,11 +2531,15 @@
         <v>317.06655499999999</v>
       </c>
       <c r="S24" s="10">
-        <f t="shared" si="1"/>
-        <v>-8.6688999863646028E-5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>8.6688999863646028E-5</v>
+      </c>
+      <c r="T24" s="13">
+        <f t="shared" si="1"/>
+        <v>317.04950475333328</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -2495,11 +2595,15 @@
         <v>3971.0111193500002</v>
       </c>
       <c r="S25" s="10">
-        <f t="shared" si="1"/>
-        <v>-1.2868714307381342E-5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.2868714307381342E-5</v>
+      </c>
+      <c r="T25" s="13">
+        <f t="shared" si="1"/>
+        <v>3970.9686125660005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -2555,11 +2659,15 @@
         <v>767.4007231999999</v>
       </c>
       <c r="S26" s="10">
-        <f t="shared" si="1"/>
-        <v>1.7928410695880433E-6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-1.7928410695880433E-6</v>
+      </c>
+      <c r="T26" s="13">
+        <f t="shared" si="1"/>
+        <v>767.40467120800008</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -2615,11 +2723,15 @@
         <v>658.36414488000003</v>
       </c>
       <c r="S27" s="10">
-        <f t="shared" si="1"/>
-        <v>4.1344898684025756E-8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-4.1344898684025756E-8</v>
+      </c>
+      <c r="T27" s="13">
+        <f t="shared" si="1"/>
+        <v>658.35965605800016</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -2675,11 +2787,15 @@
         <v>2185.01217726</v>
       </c>
       <c r="S28" s="10">
-        <f t="shared" si="1"/>
-        <v>-1.5899753602053595E-6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.5899753602053595E-6</v>
+      </c>
+      <c r="T28" s="13">
+        <f t="shared" si="1"/>
+        <v>2185.0100156359999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -2735,11 +2851,15 @@
         <v>1712.1210499399999</v>
       </c>
       <c r="S29" s="10">
-        <f t="shared" si="1"/>
-        <v>-4.9044728368680601E-6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>4.9044728368680601E-6</v>
+      </c>
+      <c r="T29" s="13">
+        <f t="shared" si="1"/>
+        <v>1712.118486204</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -2795,11 +2915,15 @@
         <v>776.63214551999999</v>
       </c>
       <c r="S30" s="10">
-        <f t="shared" si="1"/>
-        <v>-3.6202480594534782E-7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>3.6202480594534782E-7</v>
+      </c>
+      <c r="T30" s="13">
+        <f t="shared" si="1"/>
+        <v>776.63408800599984</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -2855,11 +2979,15 @@
         <v>10.3034391</v>
       </c>
       <c r="S31" s="10">
-        <f t="shared" si="1"/>
-        <v>1.2537404177813826E-5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-1.2537404177813826E-5</v>
+      </c>
+      <c r="T31" s="13">
+        <f t="shared" si="1"/>
+        <v>10.302576941999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -2915,11 +3043,15 @@
         <v>5172.6248608199994</v>
       </c>
       <c r="S32" s="10">
-        <f t="shared" si="1"/>
-        <v>7.5374247453749852E-7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-7.5374247453749852E-7</v>
+      </c>
+      <c r="T32" s="13">
+        <f t="shared" si="1"/>
+        <v>5172.6297047620001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -2975,11 +3107,15 @@
         <v>24.468666439999996</v>
       </c>
       <c r="S33" s="10">
-        <f t="shared" si="1"/>
-        <v>9.4609200233776149E-5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-9.4609200233776149E-5</v>
+      </c>
+      <c r="T33" s="13">
+        <f t="shared" si="1"/>
+        <v>24.470614558666671</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -3035,11 +3171,15 @@
         <v>107.33019479000001</v>
       </c>
       <c r="S34" s="10">
-        <f t="shared" si="1"/>
-        <v>-3.7230109240036202E-6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>3.7230109240036202E-6</v>
+      </c>
+      <c r="T34" s="13">
+        <f t="shared" si="1"/>
+        <v>107.32984462</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -3095,11 +3235,15 @@
         <v>87.58028483999999</v>
       </c>
       <c r="S35" s="10">
-        <f t="shared" si="1"/>
-        <v>3.8639623540476455E-5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-3.8639623540476455E-5</v>
+      </c>
+      <c r="T35" s="13">
+        <f t="shared" si="1"/>
+        <v>87.579894618000012</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -3155,11 +3299,15 @@
         <v>3.2110539999999999</v>
       </c>
       <c r="S36" s="10">
-        <f t="shared" si="1"/>
-        <v>4.2911507902977566E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-4.2911507902977566E-3</v>
+      </c>
+      <c r="T36" s="13">
+        <f t="shared" si="1"/>
+        <v>3.2196534240000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -3215,11 +3363,15 @@
         <v>5360.4558770000003</v>
       </c>
       <c r="S37" s="10">
-        <f t="shared" si="1"/>
-        <v>-4.5317043350158151E-8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>4.5317043350158151E-8</v>
+      </c>
+      <c r="T37" s="13">
+        <f t="shared" si="1"/>
+        <v>5360.4561496240003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -3275,11 +3427,15 @@
         <v>2050.4213154600002</v>
       </c>
       <c r="S38" s="10">
-        <f t="shared" si="1"/>
-        <v>-1.0758434652177802E-6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.0758434652177802E-6</v>
+      </c>
+      <c r="T38" s="13">
+        <f t="shared" si="1"/>
+        <v>2050.4194430213333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -3335,11 +3491,15 @@
         <v>1853.35909388</v>
       </c>
       <c r="S39" s="10">
-        <f t="shared" si="1"/>
-        <v>3.4190451031043545E-6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-3.4190451031043545E-6</v>
+      </c>
+      <c r="T39" s="13">
+        <f t="shared" si="1"/>
+        <v>1853.3619439359998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -3395,11 +3555,15 @@
         <v>164.64766559999998</v>
       </c>
       <c r="S40" s="10">
-        <f t="shared" si="1"/>
-        <v>-3.577038666812809E-5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>3.577038666812809E-5</v>
+      </c>
+      <c r="T40" s="13">
+        <f t="shared" si="1"/>
+        <v>164.64360587866668</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
@@ -3455,11 +3619,15 @@
         <v>1020.0625214400001</v>
       </c>
       <c r="S41" s="10">
-        <f t="shared" si="1"/>
-        <v>-7.417393987983148E-7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>7.417393987983148E-7</v>
+      </c>
+      <c r="T41" s="13">
+        <f t="shared" si="1"/>
+        <v>1020.0583168253336</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -3515,11 +3683,15 @@
         <v>60.744241580000001</v>
       </c>
       <c r="S42" s="10">
-        <f t="shared" si="1"/>
-        <v>1.0426502008985786E-4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-1.0426502008985786E-4</v>
+      </c>
+      <c r="T42" s="13">
+        <f t="shared" si="1"/>
+        <v>60.747816053333324</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
@@ -3575,11 +3747,15 @@
         <v>4058.9808677200003</v>
       </c>
       <c r="S43" s="10">
-        <f t="shared" si="1"/>
-        <v>3.4991037138031367E-7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-3.4991037138031367E-7</v>
+      </c>
+      <c r="T43" s="13">
+        <f t="shared" si="1"/>
+        <v>4058.9813610739993</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
@@ -3635,11 +3811,15 @@
         <v>1884.4870057999999</v>
       </c>
       <c r="S44" s="10">
-        <f t="shared" si="1"/>
-        <v>6.2489115626457491E-7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-6.2489115626457491E-7</v>
+      </c>
+      <c r="T44" s="13">
+        <f t="shared" si="1"/>
+        <v>1884.4882411773333</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>64</v>
       </c>
@@ -3695,11 +3875,15 @@
         <v>1088.10719881</v>
       </c>
       <c r="S45" s="10">
-        <f t="shared" si="1"/>
-        <v>-2.3313658037730361E-6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2.3313658037730361E-6</v>
+      </c>
+      <c r="T45" s="13">
+        <f t="shared" si="1"/>
+        <v>1088.1057546313332</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>43</v>
       </c>
@@ -3755,11 +3939,15 @@
         <v>45.296428589999998</v>
       </c>
       <c r="S46" s="10">
-        <f t="shared" si="1"/>
-        <v>-1.5496889843124792E-4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.5496889843124792E-4</v>
+      </c>
+      <c r="T46" s="13">
+        <f t="shared" si="1"/>
+        <v>45.293700252666667</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>44</v>
       </c>
@@ -3815,11 +4003,15 @@
         <v>302.88270817</v>
       </c>
       <c r="S47" s="10">
-        <f t="shared" si="1"/>
-        <v>7.6825849091127301E-6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-7.6825849091127301E-6</v>
+      </c>
+      <c r="T47" s="13">
+        <f t="shared" si="1"/>
+        <v>302.88339415733338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>45</v>
       </c>
@@ -3875,11 +4067,15 @@
         <v>1.0720930099999999</v>
       </c>
       <c r="S48" s="10">
-        <f t="shared" si="1"/>
-        <v>-4.9982389184512319E-4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>4.9982389184512319E-4</v>
+      </c>
+      <c r="T48" s="13">
+        <f t="shared" si="1"/>
+        <v>1.0729768466666667</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>46</v>
       </c>
@@ -3935,11 +4131,15 @@
         <v>3.0044735</v>
       </c>
       <c r="S49" s="10">
-        <f t="shared" si="1"/>
-        <v>1.9197681343395616E-4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-1.9197681343395616E-4</v>
+      </c>
+      <c r="T49" s="13">
+        <f t="shared" si="1"/>
+        <v>3.0057258433333334</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>47</v>
       </c>
@@ -3995,11 +4195,15 @@
         <v>542.65482127999996</v>
       </c>
       <c r="S50" s="10">
-        <f t="shared" si="1"/>
-        <v>3.6154528251375948E-6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-3.6154528251375948E-6</v>
+      </c>
+      <c r="T50" s="13">
+        <f t="shared" si="1"/>
+        <v>542.65717835800001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>48</v>
       </c>
@@ -4055,11 +4259,15 @@
         <v>276.69614349</v>
       </c>
       <c r="S51" s="10">
-        <f t="shared" si="1"/>
-        <v>5.004417672163294E-6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-5.004417672163294E-6</v>
+      </c>
+      <c r="T51" s="13">
+        <f t="shared" si="1"/>
+        <v>276.69338235600003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>49</v>
       </c>
@@ -4115,11 +4323,15 @@
         <v>217.44672943</v>
       </c>
       <c r="S52" s="10">
-        <f t="shared" si="1"/>
-        <v>3.4446652725283642E-5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-3.4446652725283642E-5</v>
+      </c>
+      <c r="T52" s="13">
+        <f t="shared" si="1"/>
+        <v>217.45028141399999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>50</v>
       </c>
@@ -4175,11 +4387,15 @@
         <v>238.92025626</v>
       </c>
       <c r="S53" s="10">
-        <f t="shared" si="1"/>
-        <v>-1.0014571384264458E-5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.0014571384264458E-5</v>
+      </c>
+      <c r="T53" s="13">
+        <f t="shared" si="1"/>
+        <v>238.91591579199996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>51</v>
       </c>
@@ -4235,11 +4451,15 @@
         <v>384.66311167999993</v>
       </c>
       <c r="S54" s="10">
-        <f t="shared" si="1"/>
-        <v>2.6163638705934048E-5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-2.6163638705934048E-5</v>
+      </c>
+      <c r="T54" s="13">
+        <f t="shared" si="1"/>
+        <v>384.6702214386666</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>52</v>
       </c>
@@ -4295,11 +4515,15 @@
         <v>567.77794352000001</v>
       </c>
       <c r="S55" s="10">
-        <f t="shared" si="1"/>
-        <v>-1.0336471730278787E-5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.0336471730278787E-5</v>
+      </c>
+      <c r="T55" s="13">
+        <f t="shared" si="1"/>
+        <v>567.77146358466655</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>53</v>
       </c>
@@ -4355,11 +4579,15 @@
         <v>108.39880479999999</v>
       </c>
       <c r="S56" s="10">
-        <f t="shared" si="1"/>
-        <v>3.8484921058308419E-5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-3.8484921058308419E-5</v>
+      </c>
+      <c r="T56" s="13">
+        <f t="shared" si="1"/>
+        <v>108.40183666399999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>54</v>
       </c>
@@ -4415,11 +4643,15 @@
         <v>2698.25998617</v>
       </c>
       <c r="S57" s="10">
-        <f t="shared" si="1"/>
-        <v>-2.0948689941605886E-7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2.0948689941605886E-7</v>
+      </c>
+      <c r="T57" s="13">
+        <f t="shared" si="1"/>
+        <v>2698.2596801686668</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>55</v>
       </c>
@@ -4475,11 +4707,15 @@
         <v>2640.9425724799999</v>
       </c>
       <c r="S58" s="10">
-        <f t="shared" si="1"/>
-        <v>-7.7452709697140172E-7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>7.7452709697140172E-7</v>
+      </c>
+      <c r="T58" s="13">
+        <f t="shared" si="1"/>
+        <v>2640.9461603220002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>56</v>
       </c>
@@ -4535,11 +4771,15 @@
         <v>1688.7220322400001</v>
       </c>
       <c r="S59" s="10">
-        <f t="shared" si="1"/>
-        <v>-2.8611895459281617E-6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2.8611895459281617E-6</v>
+      </c>
+      <c r="T59" s="13">
+        <f t="shared" si="1"/>
+        <v>1688.719739257333</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>57</v>
       </c>
@@ -4595,11 +4835,15 @@
         <v>1601.7873133600001</v>
       </c>
       <c r="S60" s="10">
-        <f t="shared" si="1"/>
-        <v>-1.7173720264928597E-6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.7173720264928597E-6</v>
+      </c>
+      <c r="T60" s="13">
+        <f t="shared" si="1"/>
+        <v>1601.7833172753333</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>58</v>
       </c>
@@ -4655,11 +4899,15 @@
         <v>103.68433040000001</v>
       </c>
       <c r="S61" s="10">
-        <f t="shared" si="1"/>
-        <v>-6.3674443499654135E-6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>6.3674443499654135E-6</v>
+      </c>
+      <c r="T61" s="13">
+        <f t="shared" si="1"/>
+        <v>103.67977827799999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>66</v>
       </c>
@@ -4715,11 +4963,15 @@
         <v>253.08210800999998</v>
       </c>
       <c r="S62" s="10">
-        <f t="shared" si="1"/>
-        <v>2.8632127768161227E-6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-2.8632127768161227E-6</v>
+      </c>
+      <c r="T62" s="13">
+        <f t="shared" si="1"/>
+        <v>253.08233653866668</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>59</v>
       </c>
@@ -4775,11 +5027,15 @@
         <v>3023.4676600800003</v>
       </c>
       <c r="S63" s="10">
-        <f t="shared" si="1"/>
-        <v>6.1717209769286996E-8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-6.1717209769286996E-8</v>
+      </c>
+      <c r="T63" s="13">
+        <f t="shared" si="1"/>
+        <v>3023.4672225653335</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>60</v>
       </c>
@@ -4835,11 +5091,15 @@
         <v>638.82333129999995</v>
       </c>
       <c r="S64" s="10">
-        <f t="shared" si="1"/>
-        <v>-1.4164499592168885E-6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.4164499592168885E-6</v>
+      </c>
+      <c r="T64" s="13">
+        <f t="shared" si="1"/>
+        <v>638.82414955599995</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>61</v>
       </c>
@@ -4895,11 +5155,15 @@
         <v>696.78218428000014</v>
       </c>
       <c r="S65" s="10">
-        <f t="shared" si="1"/>
-        <v>2.2062369605190342E-6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-2.2062369605190342E-6</v>
+      </c>
+      <c r="T65" s="13">
+        <f t="shared" si="1"/>
+        <v>696.78239702066662</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>62</v>
       </c>
@@ -4955,11 +5219,15 @@
         <v>630.23738880000008</v>
       </c>
       <c r="S66" s="10">
-        <f t="shared" si="1"/>
-        <v>4.105928053374148E-6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>-4.105928053374148E-6</v>
+      </c>
+      <c r="T66" s="13">
+        <f t="shared" si="1"/>
+        <v>630.23792834666665</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>63</v>
       </c>
@@ -5015,11 +5283,15 @@
         <v>754.30498562000002</v>
       </c>
       <c r="S67" s="10">
-        <f t="shared" si="1"/>
-        <v>8.9114618424985555E-6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" ref="S67" si="2">(R67-D67)/D67</f>
+        <v>-8.9114618424985555E-6</v>
+      </c>
+      <c r="T67" s="13">
+        <f t="shared" ref="T67" si="3">AVERAGE(D67:R67)</f>
+        <v>754.31043540999985</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -5036,7 +5308,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>

</xml_diff>